<commit_message>
committing edited personal income
</commit_message>
<xml_diff>
--- a/Personal Income.xlsx
+++ b/Personal Income.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vcarlson\Documents\Data Bootcamp\Final Project\RawData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\girar\PCI_Growth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AC7A12A-B679-4FD5-90F4-669CED16E251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DECA58-8999-412A-AA0B-5F7E186E06B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{117EE1DC-CE0F-40F4-B2B0-6580F346B04E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{117EE1DC-CE0F-40F4-B2B0-6580F346B04E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -202,8 +202,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -231,8 +239,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,174 +559,174 @@
   <dimension ref="A1:AZ12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="52" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="52" width="36.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:52" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -875,7 +884,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2010</v>
       </c>
@@ -1033,7 +1042,7 @@
         <v>26328777</v>
       </c>
     </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2011</v>
       </c>
@@ -1191,7 +1200,7 @@
         <v>28786638</v>
       </c>
     </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2012</v>
       </c>
@@ -1349,7 +1358,7 @@
         <v>31199618</v>
       </c>
     </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2013</v>
       </c>
@@ -1507,7 +1516,7 @@
         <v>31240113</v>
       </c>
     </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2014</v>
       </c>
@@ -1665,7 +1674,7 @@
         <v>33549324</v>
       </c>
     </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2015</v>
       </c>
@@ -1823,7 +1832,7 @@
         <v>33761753</v>
       </c>
     </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2016</v>
       </c>
@@ -1981,7 +1990,7 @@
         <v>31908537</v>
       </c>
     </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2017</v>
       </c>
@@ -2139,7 +2148,7 @@
         <v>32918472</v>
       </c>
     </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2018</v>
       </c>
@@ -2297,7 +2306,7 @@
         <v>34690854</v>
       </c>
     </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2019</v>
       </c>
@@ -2457,5 +2466,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>